<commit_message>
Update CDD document version 1.4
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/CDD/Review.xlsx
+++ b/Software Specification/Architecture/CDD/Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Review point</t>
   </si>
@@ -55,13 +55,22 @@
   </si>
   <si>
     <t>CDD file shall be "KeyPad CDD" not "CDD"</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">init function used only when there's global variables and in my application there's no need to use it </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,67 +143,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -793,7 +759,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -825,9 +791,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -859,6 +826,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1034,14 +1002,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1052,7 +1020,7 @@
     <col min="7" max="7" width="47.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +1043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1088,13 +1056,15 @@
       <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1107,13 +1077,17 @@
       <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="105">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1126,13 +1100,15 @@
       <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1141,7 +1117,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1150,7 +1126,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1159,7 +1135,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1168,7 +1144,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1177,7 +1153,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1186,7 +1162,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1195,7 +1171,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1203,7 +1179,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1211,7 +1187,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1221,249 +1197,249 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="69" priority="108" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="64" priority="108" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="109" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="63" priority="109" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="110" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="62" priority="110" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="66" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="85" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="86" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="64" priority="58" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="59" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="60" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="61" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="54" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="55" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="56" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="54" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="47" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="51" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="49" priority="43" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="46" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="34" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="34" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="containsText" dxfId="29" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>